<commit_message>
Updated the gerber, picknplace and BOM files and fixed some mistakes
</commit_message>
<xml_diff>
--- a/Sparrow_V101LF_COIN_BOM.xlsx
+++ b/Sparrow_V101LF_COIN_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\hardware_dev_df\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186B7ACB-0703-4672-884B-040F0F8F5759}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE4D258-4779-4880-9F1F-2EEE6D6378C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2070" windowWidth="29040" windowHeight="15840" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Qty</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>22 uF/10V (20%)</t>
-  </si>
-  <si>
-    <t>1206</t>
   </si>
   <si>
     <t>Capacitor</t>
@@ -262,9 +259,6 @@
     <t>MOSFET N-CH </t>
   </si>
   <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
     <t>N-Channel 50V 220mA (Ta) 360mW (Ta) Surface Mount SOT-23-3</t>
   </si>
   <si>
@@ -272,6 +266,12 @@
   </si>
   <si>
     <t>RF4, RF6</t>
+  </si>
+  <si>
+    <t>N-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
   </si>
 </sst>
 </file>
@@ -516,15 +516,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -554,6 +545,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99144AAD-22C5-4B4D-A92C-45347D70963E}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,23 +889,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
+      <c r="A1" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -914,10 +914,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
@@ -933,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -952,16 +952,16 @@
         <v>7</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K3" s="9"/>
     </row>
@@ -970,7 +970,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8">
         <v>4</v>
@@ -978,19 +978,19 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K4" s="9"/>
     </row>
@@ -999,7 +999,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="8">
         <v>5</v>
@@ -1007,19 +1007,19 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="24" t="s">
         <v>13</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>14</v>
       </c>
       <c r="K5" s="9"/>
     </row>
@@ -1028,7 +1028,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -1036,19 +1036,19 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="9"/>
     </row>
@@ -1057,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="8">
         <v>2</v>
@@ -1065,10 +1065,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -1080,7 +1080,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="9">
         <v>8</v>
@@ -1088,19 +1088,19 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="9"/>
     </row>
@@ -1109,31 +1109,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8">
         <v>1</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="F9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="16" t="s">
+      <c r="I9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>21</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>22</v>
       </c>
       <c r="K9" s="9"/>
     </row>
@@ -1142,29 +1142,29 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>25</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>26</v>
       </c>
       <c r="K10" s="8"/>
     </row>
@@ -1173,34 +1173,34 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="F11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="I11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1208,31 +1208,31 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="I12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="24" t="s">
         <v>34</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>35</v>
       </c>
       <c r="K12" s="9"/>
     </row>
@@ -1241,7 +1241,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
@@ -1249,22 +1249,22 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="28" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1272,166 +1272,168 @@
         <v>12</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="8">
         <v>2</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>51</v>
-      </c>
       <c r="H14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="37">
+        <v>13</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="39">
+        <v>1</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40">
-        <v>13</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="42">
-        <v>1</v>
-      </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="43" t="s">
+      <c r="G15" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="K15" s="45"/>
+      <c r="I15" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="42"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="21">
         <v>3</v>
       </c>
       <c r="D16" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="G16" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="27" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="37"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="37"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="34"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="37"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="37"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
-      <c r="I21" s="35"/>
-      <c r="K21" s="37"/>
+      <c r="I21" s="32"/>
+      <c r="K21" s="34"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>